<commit_message>
added code for sample app in flutter
</commit_message>
<xml_diff>
--- a/.Net Full Stack with I & F Program Planner.xlsx
+++ b/.Net Full Stack with I & F Program Planner.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEVEL UP SOLUTIONS 1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEVEL UP SOLUTIONS 1\Desktop\Dot-Net-Training-ITC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711C28DC-C748-4121-9401-C01397048B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878E8242-0636-43F9-BFD5-0688B25A672E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -411,7 +411,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -451,6 +451,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC4FE98"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -519,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -561,9 +567,6 @@
     <xf numFmtId="20" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -582,7 +585,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -595,18 +598,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -614,9 +629,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -918,8 +930,8 @@
   </sheetPr>
   <dimension ref="A1:I136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C70" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83:E85"/>
+    <sheetView tabSelected="1" topLeftCell="C91" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E103" sqref="E103:E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,22 +977,22 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="29">
         <v>1</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="28">
         <v>44798</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>50</v>
       </c>
       <c r="G2" s="9" t="s">
@@ -994,12 +1006,12 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="17"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="16"/>
       <c r="E3" s="30"/>
-      <c r="F3" s="20"/>
+      <c r="F3" s="19"/>
       <c r="G3" s="3" t="s">
         <v>94</v>
       </c>
@@ -1011,12 +1023,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="18"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="17"/>
       <c r="E4" s="30"/>
-      <c r="F4" s="20"/>
+      <c r="F4" s="19"/>
       <c r="G4" s="5" t="s">
         <v>97</v>
       </c>
@@ -1028,22 +1040,22 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26">
+      <c r="A5" s="29">
         <v>2</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="28">
         <v>44799</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="20"/>
+      <c r="F5" s="19"/>
       <c r="G5" s="9" t="s">
         <v>91</v>
       </c>
@@ -1055,12 +1067,12 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="17"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="30"/>
-      <c r="F6" s="20"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="3" t="s">
         <v>94</v>
       </c>
@@ -1072,12 +1084,12 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="18"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="30"/>
-      <c r="F7" s="20"/>
+      <c r="F7" s="19"/>
       <c r="G7" s="5" t="s">
         <v>97</v>
       </c>
@@ -1089,22 +1101,22 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26">
+      <c r="A8" s="29">
         <v>3</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="28">
         <v>44802</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="20"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="9" t="s">
         <v>91</v>
       </c>
@@ -1116,12 +1128,12 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="15"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="30"/>
-      <c r="F9" s="21"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="3" t="s">
         <v>94</v>
       </c>
@@ -1133,12 +1145,12 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="15"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="30"/>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="18" t="s">
         <v>51</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -1152,22 +1164,22 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26">
+      <c r="A11" s="29">
         <v>4</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="28">
         <v>44803</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="20"/>
+      <c r="F11" s="19"/>
       <c r="G11" s="9" t="s">
         <v>91</v>
       </c>
@@ -1179,12 +1191,12 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="15"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="30"/>
-      <c r="F12" s="20"/>
+      <c r="F12" s="19"/>
       <c r="G12" s="3" t="s">
         <v>94</v>
       </c>
@@ -1196,14 +1208,14 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="15" t="s">
+      <c r="A13" s="29"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="21" t="s">
         <v>67</v>
       </c>
       <c r="E13" s="30"/>
-      <c r="F13" s="20"/>
+      <c r="F13" s="19"/>
       <c r="G13" s="5" t="s">
         <v>97</v>
       </c>
@@ -1215,20 +1227,20 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26">
+      <c r="A14" s="29">
         <v>5</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="28">
         <v>44805</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15" t="s">
+      <c r="D14" s="21"/>
+      <c r="E14" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="20"/>
+      <c r="F14" s="19"/>
       <c r="G14" s="9" t="s">
         <v>91</v>
       </c>
@@ -1240,12 +1252,12 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="20"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="19"/>
       <c r="G15" s="3" t="s">
         <v>94</v>
       </c>
@@ -1257,12 +1269,12 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="21"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="5" t="s">
         <v>97</v>
       </c>
@@ -1274,22 +1286,22 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="26">
+      <c r="A17" s="29">
         <v>6</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="28">
         <v>44806</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="F17" s="18" t="s">
         <v>52</v>
       </c>
       <c r="G17" s="9" t="s">
@@ -1303,12 +1315,12 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="17"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="30"/>
-      <c r="F18" s="20"/>
+      <c r="F18" s="19"/>
       <c r="G18" s="3" t="s">
         <v>94</v>
       </c>
@@ -1320,12 +1332,12 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="17"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="16"/>
       <c r="E19" s="30"/>
-      <c r="F19" s="20"/>
+      <c r="F19" s="19"/>
       <c r="G19" s="5" t="s">
         <v>97</v>
       </c>
@@ -1337,12 +1349,12 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="18"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="30"/>
-      <c r="F20" s="20"/>
+      <c r="F20" s="19"/>
       <c r="G20" s="10" t="s">
         <v>101</v>
       </c>
@@ -1354,22 +1366,22 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26">
+      <c r="A21" s="29">
         <v>7</v>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="28">
         <v>44809</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="20"/>
+      <c r="F21" s="19"/>
       <c r="G21" s="9" t="s">
         <v>91</v>
       </c>
@@ -1381,12 +1393,12 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="20"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="19"/>
       <c r="G22" s="3" t="s">
         <v>94</v>
       </c>
@@ -1398,12 +1410,12 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="20"/>
+      <c r="A23" s="29"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="19"/>
       <c r="G23" s="5" t="s">
         <v>97</v>
       </c>
@@ -1415,22 +1427,22 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="26">
+      <c r="A24" s="29">
         <v>8</v>
       </c>
-      <c r="B24" s="27">
+      <c r="B24" s="28">
         <v>44810</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="20"/>
+      <c r="F24" s="19"/>
       <c r="G24" s="9" t="s">
         <v>91</v>
       </c>
@@ -1442,12 +1454,12 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="20"/>
+      <c r="A25" s="29"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="19"/>
       <c r="G25" s="3" t="s">
         <v>94</v>
       </c>
@@ -1459,12 +1471,12 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="20"/>
+      <c r="A26" s="29"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="19"/>
       <c r="G26" s="5" t="s">
         <v>97</v>
       </c>
@@ -1476,20 +1488,20 @@
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26">
+      <c r="A27" s="29">
         <v>9</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="28">
         <v>44811</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15" t="s">
+      <c r="D27" s="21"/>
+      <c r="E27" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="20"/>
+      <c r="F27" s="19"/>
       <c r="G27" s="9" t="s">
         <v>91</v>
       </c>
@@ -1501,12 +1513,12 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="20"/>
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="19"/>
       <c r="G28" s="3" t="s">
         <v>94</v>
       </c>
@@ -1518,12 +1530,12 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="20"/>
+      <c r="A29" s="29"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="19"/>
       <c r="G29" s="5" t="s">
         <v>97</v>
       </c>
@@ -1535,12 +1547,12 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="20"/>
+      <c r="A30" s="29"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="19"/>
       <c r="G30" s="10" t="s">
         <v>101</v>
       </c>
@@ -1552,20 +1564,20 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="26">
+      <c r="A31" s="29">
         <v>10</v>
       </c>
-      <c r="B31" s="27">
+      <c r="B31" s="28">
         <v>44812</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="20"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="19"/>
       <c r="G31" s="9" t="s">
         <v>91</v>
       </c>
@@ -1577,12 +1589,12 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="20"/>
+      <c r="A32" s="29"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="19"/>
       <c r="G32" s="3" t="s">
         <v>94</v>
       </c>
@@ -1594,12 +1606,12 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="20"/>
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="19"/>
       <c r="G33" s="14" t="s">
         <v>97</v>
       </c>
@@ -1640,22 +1652,22 @@
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="26">
+      <c r="A35" s="29">
         <v>11</v>
       </c>
-      <c r="B35" s="27">
+      <c r="B35" s="28">
         <v>44813</v>
       </c>
-      <c r="C35" s="31" t="s">
+      <c r="C35" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="E35" s="33" t="s">
+      <c r="E35" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F35" s="19" t="s">
+      <c r="F35" s="18" t="s">
         <v>53</v>
       </c>
       <c r="G35" s="9" t="s">
@@ -1669,12 +1681,12 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="26"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="20"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="19"/>
       <c r="G36" s="3" t="s">
         <v>94</v>
       </c>
@@ -1686,12 +1698,12 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="26"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="20"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="19"/>
       <c r="G37" s="5" t="s">
         <v>97</v>
       </c>
@@ -1703,12 +1715,12 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="26"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="20"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="19"/>
       <c r="G38" s="10" t="s">
         <v>101</v>
       </c>
@@ -1720,20 +1732,20 @@
       </c>
     </row>
     <row r="39" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="26">
+      <c r="A39" s="29">
         <v>12</v>
       </c>
-      <c r="B39" s="27">
+      <c r="B39" s="28">
         <v>44816</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="21"/>
-      <c r="E39" s="33" t="s">
+      <c r="D39" s="20"/>
+      <c r="E39" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="F39" s="20"/>
+      <c r="F39" s="19"/>
       <c r="G39" s="9" t="s">
         <v>91</v>
       </c>
@@ -1745,14 +1757,14 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="26"/>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="19" t="s">
+      <c r="A40" s="29"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E40" s="33"/>
-      <c r="F40" s="20"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="19"/>
       <c r="G40" s="3" t="s">
         <v>94</v>
       </c>
@@ -1764,12 +1776,12 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="26"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="20"/>
+      <c r="A41" s="29"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="19"/>
       <c r="G41" s="5" t="s">
         <v>97</v>
       </c>
@@ -1781,20 +1793,20 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="26">
+      <c r="A42" s="29">
         <v>13</v>
       </c>
-      <c r="B42" s="27">
+      <c r="B42" s="28">
         <v>44817</v>
       </c>
-      <c r="C42" s="26" t="s">
+      <c r="C42" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="33" t="s">
+      <c r="D42" s="19"/>
+      <c r="E42" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F42" s="20"/>
+      <c r="F42" s="19"/>
       <c r="G42" s="9" t="s">
         <v>91</v>
       </c>
@@ -1806,12 +1818,12 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="26"/>
-      <c r="B43" s="26"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="20"/>
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="19"/>
       <c r="G43" s="3" t="s">
         <v>94</v>
       </c>
@@ -1823,12 +1835,12 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="26"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="33"/>
-      <c r="F44" s="21"/>
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="20"/>
       <c r="G44" s="5" t="s">
         <v>97</v>
       </c>
@@ -1840,22 +1852,22 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="26">
+      <c r="A45" s="29">
         <v>14</v>
       </c>
-      <c r="B45" s="27">
+      <c r="B45" s="28">
         <v>44818</v>
       </c>
-      <c r="C45" s="29" t="s">
+      <c r="C45" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="19" t="s">
+      <c r="D45" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="E45" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="F45" s="19" t="s">
+      <c r="F45" s="18" t="s">
         <v>54</v>
       </c>
       <c r="G45" s="9" t="s">
@@ -1869,12 +1881,12 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="20"/>
+      <c r="A46" s="29"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="19"/>
       <c r="G46" s="3" t="s">
         <v>94</v>
       </c>
@@ -1886,14 +1898,14 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="19" t="s">
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="E47" s="15"/>
-      <c r="F47" s="20"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="19"/>
       <c r="G47" s="5" t="s">
         <v>97</v>
       </c>
@@ -1905,12 +1917,12 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="20"/>
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="19"/>
       <c r="G48" s="10" t="s">
         <v>101</v>
       </c>
@@ -1922,22 +1934,22 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="26">
+      <c r="A49" s="29">
         <v>15</v>
       </c>
-      <c r="B49" s="27">
+      <c r="B49" s="28">
         <v>44819</v>
       </c>
-      <c r="C49" s="26" t="s">
+      <c r="C49" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D49" s="23" t="s">
+      <c r="D49" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="E49" s="33" t="s">
+      <c r="E49" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="F49" s="20"/>
+      <c r="F49" s="19"/>
       <c r="G49" s="9" t="s">
         <v>91</v>
       </c>
@@ -1949,12 +1961,12 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="26"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="33"/>
-      <c r="F50" s="20"/>
+      <c r="A50" s="29"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="23"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="19"/>
       <c r="G50" s="3" t="s">
         <v>94</v>
       </c>
@@ -1966,12 +1978,12 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="26"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="33"/>
-      <c r="F51" s="20"/>
+      <c r="A51" s="29"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="26"/>
+      <c r="F51" s="19"/>
       <c r="G51" s="5" t="s">
         <v>97</v>
       </c>
@@ -1983,22 +1995,22 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="26">
+      <c r="A52" s="29">
         <v>16</v>
       </c>
-      <c r="B52" s="27">
+      <c r="B52" s="28">
         <v>44820</v>
       </c>
-      <c r="C52" s="29" t="s">
+      <c r="C52" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D52" s="19" t="s">
+      <c r="D52" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="E52" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F52" s="20"/>
+      <c r="F52" s="19"/>
       <c r="G52" s="9" t="s">
         <v>91</v>
       </c>
@@ -2010,12 +2022,12 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="26"/>
-      <c r="B53" s="26"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="20"/>
+      <c r="A53" s="29"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="19"/>
       <c r="G53" s="3" t="s">
         <v>94</v>
       </c>
@@ -2027,12 +2039,12 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="26"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="15"/>
-      <c r="F54" s="20"/>
+      <c r="A54" s="29"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="21"/>
+      <c r="F54" s="19"/>
       <c r="G54" s="5" t="s">
         <v>97</v>
       </c>
@@ -2044,12 +2056,12 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="26"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="15"/>
-      <c r="F55" s="20"/>
+      <c r="A55" s="29"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="21"/>
+      <c r="F55" s="19"/>
       <c r="G55" s="10" t="s">
         <v>101</v>
       </c>
@@ -2061,22 +2073,22 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="26">
+      <c r="A56" s="29">
         <v>17</v>
       </c>
-      <c r="B56" s="27">
+      <c r="B56" s="28">
         <v>44823</v>
       </c>
-      <c r="C56" s="26" t="s">
+      <c r="C56" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="19" t="s">
+      <c r="D56" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="E56" s="15" t="s">
+      <c r="E56" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F56" s="20"/>
+      <c r="F56" s="19"/>
       <c r="G56" s="9" t="s">
         <v>91</v>
       </c>
@@ -2088,12 +2100,12 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="26"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="20"/>
+      <c r="A57" s="29"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="19"/>
       <c r="G57" s="3" t="s">
         <v>94</v>
       </c>
@@ -2105,12 +2117,12 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="26"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="15"/>
-      <c r="F58" s="20"/>
+      <c r="A58" s="29"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="19"/>
       <c r="G58" s="5" t="s">
         <v>97</v>
       </c>
@@ -2122,20 +2134,20 @@
       </c>
     </row>
     <row r="59" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="26">
+      <c r="A59" s="29">
         <v>18</v>
       </c>
-      <c r="B59" s="27">
+      <c r="B59" s="28">
         <v>44824</v>
       </c>
-      <c r="C59" s="26" t="s">
+      <c r="C59" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D59" s="20"/>
-      <c r="E59" s="15" t="s">
+      <c r="D59" s="19"/>
+      <c r="E59" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F59" s="20"/>
+      <c r="F59" s="19"/>
       <c r="G59" s="9" t="s">
         <v>91</v>
       </c>
@@ -2147,12 +2159,12 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="26"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="20"/>
+      <c r="A60" s="29"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="21"/>
+      <c r="F60" s="19"/>
       <c r="G60" s="3" t="s">
         <v>94</v>
       </c>
@@ -2164,12 +2176,12 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="26"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="21"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="20"/>
+      <c r="A61" s="29"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="21"/>
+      <c r="F61" s="19"/>
       <c r="G61" s="5" t="s">
         <v>97</v>
       </c>
@@ -2181,22 +2193,22 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="26">
+      <c r="A62" s="29">
         <v>19</v>
       </c>
-      <c r="B62" s="27">
+      <c r="B62" s="28">
         <v>44825</v>
       </c>
-      <c r="C62" s="29" t="s">
+      <c r="C62" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D62" s="19" t="s">
+      <c r="D62" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E62" s="15" t="s">
+      <c r="E62" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F62" s="20"/>
+      <c r="F62" s="19"/>
       <c r="G62" s="9" t="s">
         <v>91</v>
       </c>
@@ -2208,12 +2220,12 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="26"/>
-      <c r="B63" s="26"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="20"/>
+      <c r="A63" s="29"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="19"/>
       <c r="G63" s="3" t="s">
         <v>94</v>
       </c>
@@ -2225,12 +2237,12 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="26"/>
-      <c r="B64" s="26"/>
-      <c r="C64" s="29"/>
-      <c r="D64" s="20"/>
-      <c r="E64" s="15"/>
-      <c r="F64" s="20"/>
+      <c r="A64" s="29"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="21"/>
+      <c r="F64" s="19"/>
       <c r="G64" s="5" t="s">
         <v>97</v>
       </c>
@@ -2242,12 +2254,12 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="26"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="29"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="15"/>
-      <c r="F65" s="20"/>
+      <c r="A65" s="29"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="21"/>
+      <c r="F65" s="19"/>
       <c r="G65" s="10" t="s">
         <v>101</v>
       </c>
@@ -2259,20 +2271,20 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="26">
+      <c r="A66" s="29">
         <v>20</v>
       </c>
-      <c r="B66" s="27">
+      <c r="B66" s="28">
         <v>44826</v>
       </c>
-      <c r="C66" s="26" t="s">
+      <c r="C66" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D66" s="20"/>
-      <c r="E66" s="33" t="s">
+      <c r="D66" s="19"/>
+      <c r="E66" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F66" s="20"/>
+      <c r="F66" s="19"/>
       <c r="G66" s="9" t="s">
         <v>91</v>
       </c>
@@ -2284,12 +2296,12 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="26"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="26"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="33"/>
-      <c r="F67" s="20"/>
+      <c r="A67" s="29"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="26"/>
+      <c r="F67" s="19"/>
       <c r="G67" s="3" t="s">
         <v>94</v>
       </c>
@@ -2301,12 +2313,12 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="26"/>
-      <c r="B68" s="26"/>
-      <c r="C68" s="26"/>
-      <c r="D68" s="21"/>
-      <c r="E68" s="33"/>
-      <c r="F68" s="21"/>
+      <c r="A68" s="29"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="20"/>
       <c r="G68" s="5" t="s">
         <v>97</v>
       </c>
@@ -2318,22 +2330,22 @@
       </c>
     </row>
     <row r="69" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="26">
+      <c r="A69" s="29">
         <v>21</v>
       </c>
-      <c r="B69" s="27">
+      <c r="B69" s="28">
         <v>44827</v>
       </c>
-      <c r="C69" s="31" t="s">
+      <c r="C69" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D69" s="19" t="s">
+      <c r="D69" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="E69" s="33" t="s">
+      <c r="E69" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="F69" s="19" t="s">
+      <c r="F69" s="18" t="s">
         <v>55</v>
       </c>
       <c r="G69" s="9" t="s">
@@ -2347,12 +2359,12 @@
       </c>
     </row>
     <row r="70" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="26"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="33"/>
-      <c r="F70" s="20"/>
+      <c r="A70" s="29"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="19"/>
       <c r="G70" s="3" t="s">
         <v>94</v>
       </c>
@@ -2364,12 +2376,12 @@
       </c>
     </row>
     <row r="71" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="26"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="31"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="33"/>
-      <c r="F71" s="21"/>
+      <c r="A71" s="29"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="34"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="26"/>
+      <c r="F71" s="20"/>
       <c r="G71" s="14" t="s">
         <v>97</v>
       </c>
@@ -2410,22 +2422,22 @@
       </c>
     </row>
     <row r="73" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="26">
+      <c r="A73" s="29">
         <v>22</v>
       </c>
-      <c r="B73" s="27">
+      <c r="B73" s="28">
         <v>44830</v>
       </c>
-      <c r="C73" s="26" t="s">
+      <c r="C73" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D73" s="22" t="s">
+      <c r="D73" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="E73" s="22" t="s">
+      <c r="E73" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="F73" s="19" t="s">
+      <c r="F73" s="18" t="s">
         <v>106</v>
       </c>
       <c r="G73" s="9" t="s">
@@ -2439,12 +2451,12 @@
       </c>
     </row>
     <row r="74" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="26"/>
-      <c r="B74" s="26"/>
-      <c r="C74" s="26"/>
-      <c r="D74" s="22"/>
-      <c r="E74" s="22"/>
-      <c r="F74" s="20"/>
+      <c r="A74" s="29"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="25"/>
+      <c r="E74" s="25"/>
+      <c r="F74" s="19"/>
       <c r="G74" s="3" t="s">
         <v>94</v>
       </c>
@@ -2456,14 +2468,14 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="26"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="26"/>
+      <c r="A75" s="29"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
       <c r="D75" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="E75" s="22"/>
-      <c r="F75" s="20"/>
+      <c r="E75" s="25"/>
+      <c r="F75" s="19"/>
       <c r="G75" s="5" t="s">
         <v>97</v>
       </c>
@@ -2475,22 +2487,22 @@
       </c>
     </row>
     <row r="76" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="26">
+      <c r="A76" s="29">
         <v>23</v>
       </c>
-      <c r="B76" s="27">
+      <c r="B76" s="28">
         <v>44831</v>
       </c>
-      <c r="C76" s="26" t="s">
+      <c r="C76" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D76" s="20" t="s">
+      <c r="D76" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="E76" s="33" t="s">
+      <c r="E76" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="F76" s="22" t="s">
+      <c r="F76" s="25" t="s">
         <v>56</v>
       </c>
       <c r="G76" s="9" t="s">
@@ -2504,12 +2516,12 @@
       </c>
     </row>
     <row r="77" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="26"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="26"/>
-      <c r="D77" s="20"/>
-      <c r="E77" s="34"/>
-      <c r="F77" s="22"/>
+      <c r="A77" s="29"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="36"/>
+      <c r="F77" s="25"/>
       <c r="G77" s="3" t="s">
         <v>94</v>
       </c>
@@ -2521,12 +2533,12 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="26"/>
-      <c r="B78" s="26"/>
-      <c r="C78" s="26"/>
-      <c r="D78" s="21"/>
-      <c r="E78" s="34"/>
-      <c r="F78" s="22"/>
+      <c r="A78" s="29"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="36"/>
+      <c r="F78" s="25"/>
       <c r="G78" s="5" t="s">
         <v>97</v>
       </c>
@@ -2538,22 +2550,22 @@
       </c>
     </row>
     <row r="79" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="26">
+      <c r="A79" s="29">
         <v>24</v>
       </c>
-      <c r="B79" s="27">
+      <c r="B79" s="28">
         <v>44832</v>
       </c>
-      <c r="C79" s="29" t="s">
+      <c r="C79" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D79" s="19" t="s">
+      <c r="D79" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="E79" s="33" t="s">
+      <c r="E79" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="F79" s="20" t="s">
+      <c r="F79" s="19" t="s">
         <v>57</v>
       </c>
       <c r="G79" s="9" t="s">
@@ -2567,12 +2579,12 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="26"/>
-      <c r="B80" s="26"/>
-      <c r="C80" s="32"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="33"/>
-      <c r="F80" s="20"/>
+      <c r="A80" s="29"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="35"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="26"/>
+      <c r="F80" s="19"/>
       <c r="G80" s="3" t="s">
         <v>94</v>
       </c>
@@ -2584,12 +2596,12 @@
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="26"/>
-      <c r="B81" s="26"/>
-      <c r="C81" s="32"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="33"/>
-      <c r="F81" s="20"/>
+      <c r="A81" s="29"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="35"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="26"/>
+      <c r="F81" s="19"/>
       <c r="G81" s="5" t="s">
         <v>97</v>
       </c>
@@ -2601,12 +2613,12 @@
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="26"/>
-      <c r="B82" s="26"/>
-      <c r="C82" s="32"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="33"/>
-      <c r="F82" s="20"/>
+      <c r="A82" s="29"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="35"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="26"/>
+      <c r="F82" s="19"/>
       <c r="G82" s="10" t="s">
         <v>101</v>
       </c>
@@ -2618,22 +2630,22 @@
       </c>
     </row>
     <row r="83" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="26">
+      <c r="A83" s="29">
         <v>25</v>
       </c>
-      <c r="B83" s="27">
+      <c r="B83" s="28">
         <v>44833</v>
       </c>
-      <c r="C83" s="26" t="s">
+      <c r="C83" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D83" s="20" t="s">
+      <c r="D83" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="E83" s="22" t="s">
+      <c r="E83" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="F83" s="20"/>
+      <c r="F83" s="19"/>
       <c r="G83" s="9" t="s">
         <v>91</v>
       </c>
@@ -2645,12 +2657,12 @@
       </c>
     </row>
     <row r="84" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="26"/>
-      <c r="B84" s="26"/>
-      <c r="C84" s="26"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="22"/>
-      <c r="F84" s="20"/>
+      <c r="A84" s="29"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="29"/>
+      <c r="D84" s="19"/>
+      <c r="E84" s="25"/>
+      <c r="F84" s="19"/>
       <c r="G84" s="3" t="s">
         <v>94</v>
       </c>
@@ -2662,12 +2674,12 @@
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="26"/>
-      <c r="B85" s="26"/>
-      <c r="C85" s="26"/>
-      <c r="D85" s="20"/>
-      <c r="E85" s="22"/>
-      <c r="F85" s="20"/>
+      <c r="A85" s="29"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="25"/>
+      <c r="F85" s="19"/>
       <c r="G85" s="5" t="s">
         <v>97</v>
       </c>
@@ -2679,22 +2691,22 @@
       </c>
     </row>
     <row r="86" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="26">
+      <c r="A86" s="29">
         <v>26</v>
       </c>
-      <c r="B86" s="27">
+      <c r="B86" s="28">
         <v>44834</v>
       </c>
-      <c r="C86" s="29" t="s">
+      <c r="C86" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D86" s="19" t="s">
+      <c r="D86" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="E86" s="22" t="s">
+      <c r="E86" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F86" s="19" t="s">
+      <c r="F86" s="18" t="s">
         <v>58</v>
       </c>
       <c r="G86" s="9" t="s">
@@ -2708,12 +2720,12 @@
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="26"/>
-      <c r="B87" s="26"/>
-      <c r="C87" s="29"/>
-      <c r="D87" s="20"/>
-      <c r="E87" s="22"/>
-      <c r="F87" s="20"/>
+      <c r="A87" s="29"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="31"/>
+      <c r="D87" s="19"/>
+      <c r="E87" s="27"/>
+      <c r="F87" s="19"/>
       <c r="G87" s="3" t="s">
         <v>94</v>
       </c>
@@ -2725,12 +2737,12 @@
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="26"/>
-      <c r="B88" s="26"/>
-      <c r="C88" s="29"/>
-      <c r="D88" s="20"/>
-      <c r="E88" s="22"/>
-      <c r="F88" s="20"/>
+      <c r="A88" s="29"/>
+      <c r="B88" s="29"/>
+      <c r="C88" s="31"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="27"/>
+      <c r="F88" s="19"/>
       <c r="G88" s="5" t="s">
         <v>97</v>
       </c>
@@ -2742,12 +2754,12 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="26"/>
-      <c r="B89" s="26"/>
-      <c r="C89" s="29"/>
-      <c r="D89" s="20"/>
-      <c r="E89" s="22"/>
-      <c r="F89" s="20"/>
+      <c r="A89" s="29"/>
+      <c r="B89" s="29"/>
+      <c r="C89" s="31"/>
+      <c r="D89" s="19"/>
+      <c r="E89" s="27"/>
+      <c r="F89" s="19"/>
       <c r="G89" s="10" t="s">
         <v>101</v>
       </c>
@@ -2759,20 +2771,20 @@
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="26">
+      <c r="A90" s="29">
         <v>27</v>
       </c>
-      <c r="B90" s="27">
+      <c r="B90" s="28">
         <v>44837</v>
       </c>
-      <c r="C90" s="26" t="s">
+      <c r="C90" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D90" s="20"/>
-      <c r="E90" s="22" t="s">
+      <c r="D90" s="19"/>
+      <c r="E90" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="F90" s="20"/>
+      <c r="F90" s="19"/>
       <c r="G90" s="9" t="s">
         <v>91</v>
       </c>
@@ -2784,12 +2796,12 @@
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="26"/>
-      <c r="B91" s="26"/>
-      <c r="C91" s="26"/>
-      <c r="D91" s="20"/>
-      <c r="E91" s="22"/>
-      <c r="F91" s="20"/>
+      <c r="A91" s="29"/>
+      <c r="B91" s="29"/>
+      <c r="C91" s="29"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="27"/>
+      <c r="F91" s="19"/>
       <c r="G91" s="3" t="s">
         <v>94</v>
       </c>
@@ -2801,12 +2813,12 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="26"/>
-      <c r="B92" s="26"/>
-      <c r="C92" s="26"/>
-      <c r="D92" s="21"/>
-      <c r="E92" s="22"/>
-      <c r="F92" s="20"/>
+      <c r="A92" s="29"/>
+      <c r="B92" s="29"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="20"/>
+      <c r="E92" s="27"/>
+      <c r="F92" s="19"/>
       <c r="G92" s="5" t="s">
         <v>97</v>
       </c>
@@ -2818,22 +2830,22 @@
       </c>
     </row>
     <row r="93" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="26">
+      <c r="A93" s="29">
         <v>28</v>
       </c>
-      <c r="B93" s="27">
+      <c r="B93" s="28">
         <v>44840</v>
       </c>
-      <c r="C93" s="26" t="s">
+      <c r="C93" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D93" s="22" t="s">
+      <c r="D93" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="E93" s="22" t="s">
+      <c r="E93" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="F93" s="20"/>
+      <c r="F93" s="19"/>
       <c r="G93" s="9" t="s">
         <v>91</v>
       </c>
@@ -2845,12 +2857,12 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="26"/>
-      <c r="B94" s="26"/>
-      <c r="C94" s="26"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="22"/>
-      <c r="F94" s="20"/>
+      <c r="A94" s="29"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="29"/>
+      <c r="D94" s="25"/>
+      <c r="E94" s="27"/>
+      <c r="F94" s="19"/>
       <c r="G94" s="3" t="s">
         <v>94</v>
       </c>
@@ -2862,12 +2874,12 @@
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="26"/>
-      <c r="B95" s="26"/>
-      <c r="C95" s="26"/>
-      <c r="D95" s="22"/>
-      <c r="E95" s="22"/>
-      <c r="F95" s="20"/>
+      <c r="A95" s="29"/>
+      <c r="B95" s="29"/>
+      <c r="C95" s="29"/>
+      <c r="D95" s="25"/>
+      <c r="E95" s="27"/>
+      <c r="F95" s="19"/>
       <c r="G95" s="5" t="s">
         <v>97</v>
       </c>
@@ -2879,22 +2891,22 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="26">
+      <c r="A96" s="29">
         <v>29</v>
       </c>
-      <c r="B96" s="27">
+      <c r="B96" s="28">
         <v>44841</v>
       </c>
-      <c r="C96" s="29" t="s">
+      <c r="C96" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D96" s="19" t="s">
+      <c r="D96" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="E96" s="26" t="s">
+      <c r="E96" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="F96" s="20"/>
+      <c r="F96" s="19"/>
       <c r="G96" s="9" t="s">
         <v>91</v>
       </c>
@@ -2906,12 +2918,12 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="26"/>
-      <c r="B97" s="26"/>
-      <c r="C97" s="29"/>
-      <c r="D97" s="20"/>
-      <c r="E97" s="26"/>
-      <c r="F97" s="20"/>
+      <c r="A97" s="29"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="31"/>
+      <c r="D97" s="19"/>
+      <c r="E97" s="32"/>
+      <c r="F97" s="19"/>
       <c r="G97" s="3" t="s">
         <v>94</v>
       </c>
@@ -2923,12 +2935,12 @@
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="26"/>
-      <c r="B98" s="26"/>
-      <c r="C98" s="29"/>
-      <c r="D98" s="20"/>
-      <c r="E98" s="26"/>
-      <c r="F98" s="20"/>
+      <c r="A98" s="29"/>
+      <c r="B98" s="29"/>
+      <c r="C98" s="31"/>
+      <c r="D98" s="19"/>
+      <c r="E98" s="32"/>
+      <c r="F98" s="19"/>
       <c r="G98" s="5" t="s">
         <v>97</v>
       </c>
@@ -2940,12 +2952,12 @@
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="26"/>
-      <c r="B99" s="26"/>
-      <c r="C99" s="29"/>
-      <c r="D99" s="20"/>
-      <c r="E99" s="26"/>
-      <c r="F99" s="20"/>
+      <c r="A99" s="29"/>
+      <c r="B99" s="29"/>
+      <c r="C99" s="31"/>
+      <c r="D99" s="19"/>
+      <c r="E99" s="32"/>
+      <c r="F99" s="19"/>
       <c r="G99" s="10" t="s">
         <v>101</v>
       </c>
@@ -2957,20 +2969,20 @@
       </c>
     </row>
     <row r="100" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="26">
+      <c r="A100" s="29">
         <v>30</v>
       </c>
-      <c r="B100" s="27">
+      <c r="B100" s="28">
         <v>44844</v>
       </c>
-      <c r="C100" s="26" t="s">
+      <c r="C100" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D100" s="20"/>
-      <c r="E100" s="22" t="s">
+      <c r="D100" s="19"/>
+      <c r="E100" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="F100" s="20"/>
+      <c r="F100" s="19"/>
       <c r="G100" s="9" t="s">
         <v>91</v>
       </c>
@@ -2982,12 +2994,12 @@
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="26"/>
-      <c r="B101" s="26"/>
-      <c r="C101" s="28"/>
-      <c r="D101" s="20"/>
-      <c r="E101" s="22"/>
-      <c r="F101" s="20"/>
+      <c r="A101" s="29"/>
+      <c r="B101" s="29"/>
+      <c r="C101" s="33"/>
+      <c r="D101" s="19"/>
+      <c r="E101" s="27"/>
+      <c r="F101" s="19"/>
       <c r="G101" s="3" t="s">
         <v>94</v>
       </c>
@@ -2999,12 +3011,12 @@
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="26"/>
-      <c r="B102" s="26"/>
-      <c r="C102" s="28"/>
-      <c r="D102" s="20"/>
-      <c r="E102" s="22"/>
-      <c r="F102" s="20"/>
+      <c r="A102" s="29"/>
+      <c r="B102" s="29"/>
+      <c r="C102" s="33"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="27"/>
+      <c r="F102" s="19"/>
       <c r="G102" s="5" t="s">
         <v>97</v>
       </c>
@@ -3016,22 +3028,22 @@
       </c>
     </row>
     <row r="103" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="26">
+      <c r="A103" s="29">
         <v>31</v>
       </c>
-      <c r="B103" s="27">
+      <c r="B103" s="28">
         <v>44845</v>
       </c>
-      <c r="C103" s="26" t="s">
+      <c r="C103" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D103" s="19" t="s">
+      <c r="D103" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="E103" s="22" t="s">
+      <c r="E103" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="F103" s="19" t="s">
+      <c r="F103" s="18" t="s">
         <v>59</v>
       </c>
       <c r="G103" s="9" t="s">
@@ -3045,12 +3057,12 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="26"/>
-      <c r="B104" s="26"/>
-      <c r="C104" s="26"/>
-      <c r="D104" s="20"/>
-      <c r="E104" s="22"/>
-      <c r="F104" s="20"/>
+      <c r="A104" s="29"/>
+      <c r="B104" s="29"/>
+      <c r="C104" s="29"/>
+      <c r="D104" s="19"/>
+      <c r="E104" s="25"/>
+      <c r="F104" s="19"/>
       <c r="G104" s="3" t="s">
         <v>94</v>
       </c>
@@ -3062,12 +3074,12 @@
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="26"/>
-      <c r="B105" s="26"/>
-      <c r="C105" s="26"/>
-      <c r="D105" s="20"/>
-      <c r="E105" s="22"/>
-      <c r="F105" s="20"/>
+      <c r="A105" s="29"/>
+      <c r="B105" s="29"/>
+      <c r="C105" s="29"/>
+      <c r="D105" s="19"/>
+      <c r="E105" s="25"/>
+      <c r="F105" s="19"/>
       <c r="G105" s="5" t="s">
         <v>97</v>
       </c>
@@ -3079,20 +3091,20 @@
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="26">
+      <c r="A106" s="29">
         <v>32</v>
       </c>
-      <c r="B106" s="27">
+      <c r="B106" s="28">
         <v>44846</v>
       </c>
-      <c r="C106" s="29" t="s">
+      <c r="C106" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D106" s="20"/>
-      <c r="E106" s="22" t="s">
+      <c r="D106" s="19"/>
+      <c r="E106" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="F106" s="20"/>
+      <c r="F106" s="19"/>
       <c r="G106" s="9" t="s">
         <v>91</v>
       </c>
@@ -3104,12 +3116,12 @@
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="26"/>
-      <c r="B107" s="26"/>
-      <c r="C107" s="29"/>
-      <c r="D107" s="20"/>
-      <c r="E107" s="22"/>
-      <c r="F107" s="20"/>
+      <c r="A107" s="29"/>
+      <c r="B107" s="29"/>
+      <c r="C107" s="31"/>
+      <c r="D107" s="19"/>
+      <c r="E107" s="25"/>
+      <c r="F107" s="19"/>
       <c r="G107" s="3" t="s">
         <v>94</v>
       </c>
@@ -3121,12 +3133,12 @@
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="26"/>
-      <c r="B108" s="26"/>
-      <c r="C108" s="29"/>
-      <c r="D108" s="20"/>
-      <c r="E108" s="22"/>
-      <c r="F108" s="20"/>
+      <c r="A108" s="29"/>
+      <c r="B108" s="29"/>
+      <c r="C108" s="31"/>
+      <c r="D108" s="19"/>
+      <c r="E108" s="25"/>
+      <c r="F108" s="19"/>
       <c r="G108" s="5" t="s">
         <v>97</v>
       </c>
@@ -3138,12 +3150,12 @@
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="26"/>
-      <c r="B109" s="26"/>
-      <c r="C109" s="29"/>
-      <c r="D109" s="20"/>
-      <c r="E109" s="22"/>
-      <c r="F109" s="20"/>
+      <c r="A109" s="29"/>
+      <c r="B109" s="29"/>
+      <c r="C109" s="31"/>
+      <c r="D109" s="19"/>
+      <c r="E109" s="25"/>
+      <c r="F109" s="19"/>
       <c r="G109" s="10" t="s">
         <v>101</v>
       </c>
@@ -3155,20 +3167,20 @@
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="26">
+      <c r="A110" s="29">
         <v>33</v>
       </c>
-      <c r="B110" s="27">
+      <c r="B110" s="28">
         <v>44847</v>
       </c>
-      <c r="C110" s="26" t="s">
+      <c r="C110" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D110" s="20"/>
-      <c r="E110" s="22" t="s">
+      <c r="D110" s="19"/>
+      <c r="E110" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F110" s="20"/>
+      <c r="F110" s="19"/>
       <c r="G110" s="9" t="s">
         <v>91</v>
       </c>
@@ -3180,12 +3192,12 @@
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="26"/>
-      <c r="B111" s="26"/>
-      <c r="C111" s="26"/>
-      <c r="D111" s="20"/>
-      <c r="E111" s="22"/>
-      <c r="F111" s="20"/>
+      <c r="A111" s="29"/>
+      <c r="B111" s="29"/>
+      <c r="C111" s="29"/>
+      <c r="D111" s="19"/>
+      <c r="E111" s="25"/>
+      <c r="F111" s="19"/>
       <c r="G111" s="3" t="s">
         <v>94</v>
       </c>
@@ -3197,12 +3209,12 @@
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="26"/>
-      <c r="B112" s="26"/>
-      <c r="C112" s="26"/>
-      <c r="D112" s="20"/>
-      <c r="E112" s="22"/>
-      <c r="F112" s="20"/>
+      <c r="A112" s="29"/>
+      <c r="B112" s="29"/>
+      <c r="C112" s="29"/>
+      <c r="D112" s="19"/>
+      <c r="E112" s="25"/>
+      <c r="F112" s="19"/>
       <c r="G112" s="5" t="s">
         <v>97</v>
       </c>
@@ -3214,20 +3226,20 @@
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="26">
+      <c r="A113" s="29">
         <v>34</v>
       </c>
-      <c r="B113" s="27">
+      <c r="B113" s="28">
         <v>44848</v>
       </c>
-      <c r="C113" s="29" t="s">
+      <c r="C113" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D113" s="20"/>
-      <c r="E113" s="22" t="s">
+      <c r="D113" s="19"/>
+      <c r="E113" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="F113" s="20"/>
+      <c r="F113" s="19"/>
       <c r="G113" s="9" t="s">
         <v>91</v>
       </c>
@@ -3239,12 +3251,12 @@
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="26"/>
-      <c r="B114" s="26"/>
-      <c r="C114" s="29"/>
-      <c r="D114" s="20"/>
-      <c r="E114" s="22"/>
-      <c r="F114" s="20"/>
+      <c r="A114" s="29"/>
+      <c r="B114" s="29"/>
+      <c r="C114" s="31"/>
+      <c r="D114" s="19"/>
+      <c r="E114" s="25"/>
+      <c r="F114" s="19"/>
       <c r="G114" s="3" t="s">
         <v>94</v>
       </c>
@@ -3256,12 +3268,12 @@
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="26"/>
-      <c r="B115" s="26"/>
-      <c r="C115" s="29"/>
-      <c r="D115" s="20"/>
-      <c r="E115" s="22"/>
-      <c r="F115" s="20"/>
+      <c r="A115" s="29"/>
+      <c r="B115" s="29"/>
+      <c r="C115" s="31"/>
+      <c r="D115" s="19"/>
+      <c r="E115" s="25"/>
+      <c r="F115" s="19"/>
       <c r="G115" s="5" t="s">
         <v>97</v>
       </c>
@@ -3273,12 +3285,12 @@
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="26"/>
-      <c r="B116" s="26"/>
-      <c r="C116" s="29"/>
-      <c r="D116" s="21"/>
-      <c r="E116" s="22"/>
-      <c r="F116" s="20"/>
+      <c r="A116" s="29"/>
+      <c r="B116" s="29"/>
+      <c r="C116" s="31"/>
+      <c r="D116" s="20"/>
+      <c r="E116" s="25"/>
+      <c r="F116" s="19"/>
       <c r="G116" s="10" t="s">
         <v>101</v>
       </c>
@@ -3290,22 +3302,22 @@
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="26">
+      <c r="A117" s="29">
         <v>35</v>
       </c>
-      <c r="B117" s="27">
+      <c r="B117" s="28">
         <v>44851</v>
       </c>
-      <c r="C117" s="26" t="s">
+      <c r="C117" s="29" t="s">
         <v>5</v>
       </c>
       <c r="D117" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E117" s="22" t="s">
+      <c r="E117" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="F117" s="20"/>
+      <c r="F117" s="19"/>
       <c r="G117" s="9" t="s">
         <v>91</v>
       </c>
@@ -3317,14 +3329,14 @@
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="26"/>
-      <c r="B118" s="26"/>
-      <c r="C118" s="26"/>
-      <c r="D118" s="19" t="s">
+      <c r="A118" s="29"/>
+      <c r="B118" s="29"/>
+      <c r="C118" s="29"/>
+      <c r="D118" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E118" s="22"/>
-      <c r="F118" s="20"/>
+      <c r="E118" s="25"/>
+      <c r="F118" s="19"/>
       <c r="G118" s="3" t="s">
         <v>94</v>
       </c>
@@ -3336,12 +3348,12 @@
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="26"/>
-      <c r="B119" s="26"/>
-      <c r="C119" s="26"/>
-      <c r="D119" s="21"/>
-      <c r="E119" s="22"/>
-      <c r="F119" s="21"/>
+      <c r="A119" s="29"/>
+      <c r="B119" s="29"/>
+      <c r="C119" s="29"/>
+      <c r="D119" s="20"/>
+      <c r="E119" s="25"/>
+      <c r="F119" s="20"/>
       <c r="G119" s="14" t="s">
         <v>97</v>
       </c>
@@ -3382,22 +3394,22 @@
       </c>
     </row>
     <row r="121" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="26">
+      <c r="A121" s="29">
         <v>36</v>
       </c>
-      <c r="B121" s="27">
+      <c r="B121" s="28">
         <v>44852</v>
       </c>
-      <c r="C121" s="26" t="s">
+      <c r="C121" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D121" s="19" t="s">
+      <c r="D121" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E121" s="19" t="s">
+      <c r="E121" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F121" s="22" t="s">
+      <c r="F121" s="25" t="s">
         <v>60</v>
       </c>
       <c r="G121" s="9" t="s">
@@ -3411,12 +3423,12 @@
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="26"/>
-      <c r="B122" s="26"/>
-      <c r="C122" s="26"/>
-      <c r="D122" s="20"/>
-      <c r="E122" s="20"/>
-      <c r="F122" s="22"/>
+      <c r="A122" s="29"/>
+      <c r="B122" s="29"/>
+      <c r="C122" s="29"/>
+      <c r="D122" s="19"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="25"/>
       <c r="G122" s="3" t="s">
         <v>94</v>
       </c>
@@ -3428,12 +3440,12 @@
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="26"/>
-      <c r="B123" s="26"/>
-      <c r="C123" s="26"/>
-      <c r="D123" s="20"/>
-      <c r="E123" s="20"/>
-      <c r="F123" s="22"/>
+      <c r="A123" s="29"/>
+      <c r="B123" s="29"/>
+      <c r="C123" s="29"/>
+      <c r="D123" s="19"/>
+      <c r="E123" s="19"/>
+      <c r="F123" s="25"/>
       <c r="G123" s="5" t="s">
         <v>97</v>
       </c>
@@ -3445,18 +3457,18 @@
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="26">
+      <c r="A124" s="29">
         <v>37</v>
       </c>
-      <c r="B124" s="27">
+      <c r="B124" s="28">
         <v>44853</v>
       </c>
-      <c r="C124" s="29" t="s">
+      <c r="C124" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D124" s="20"/>
-      <c r="E124" s="20"/>
-      <c r="F124" s="22"/>
+      <c r="D124" s="19"/>
+      <c r="E124" s="19"/>
+      <c r="F124" s="25"/>
       <c r="G124" s="9" t="s">
         <v>91</v>
       </c>
@@ -3468,12 +3480,12 @@
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="26"/>
-      <c r="B125" s="26"/>
-      <c r="C125" s="29"/>
-      <c r="D125" s="20"/>
-      <c r="E125" s="20"/>
-      <c r="F125" s="22"/>
+      <c r="A125" s="29"/>
+      <c r="B125" s="29"/>
+      <c r="C125" s="31"/>
+      <c r="D125" s="19"/>
+      <c r="E125" s="19"/>
+      <c r="F125" s="25"/>
       <c r="G125" s="9" t="s">
         <v>91</v>
       </c>
@@ -3485,12 +3497,12 @@
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A126" s="26"/>
-      <c r="B126" s="26"/>
-      <c r="C126" s="29"/>
-      <c r="D126" s="20"/>
-      <c r="E126" s="20"/>
-      <c r="F126" s="22"/>
+      <c r="A126" s="29"/>
+      <c r="B126" s="29"/>
+      <c r="C126" s="31"/>
+      <c r="D126" s="19"/>
+      <c r="E126" s="19"/>
+      <c r="F126" s="25"/>
       <c r="G126" s="3" t="s">
         <v>94</v>
       </c>
@@ -3502,12 +3514,12 @@
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" s="26"/>
-      <c r="B127" s="26"/>
-      <c r="C127" s="29"/>
-      <c r="D127" s="20"/>
-      <c r="E127" s="20"/>
-      <c r="F127" s="22"/>
+      <c r="A127" s="29"/>
+      <c r="B127" s="29"/>
+      <c r="C127" s="31"/>
+      <c r="D127" s="19"/>
+      <c r="E127" s="19"/>
+      <c r="F127" s="25"/>
       <c r="G127" s="5" t="s">
         <v>97</v>
       </c>
@@ -3519,18 +3531,18 @@
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" s="26">
+      <c r="A128" s="29">
         <v>38</v>
       </c>
-      <c r="B128" s="27">
+      <c r="B128" s="28">
         <v>44854</v>
       </c>
-      <c r="C128" s="26" t="s">
+      <c r="C128" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D128" s="20"/>
-      <c r="E128" s="20"/>
-      <c r="F128" s="22"/>
+      <c r="D128" s="19"/>
+      <c r="E128" s="19"/>
+      <c r="F128" s="25"/>
       <c r="G128" s="10" t="s">
         <v>101</v>
       </c>
@@ -3542,12 +3554,12 @@
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="26"/>
-      <c r="B129" s="26"/>
-      <c r="C129" s="26"/>
-      <c r="D129" s="20"/>
-      <c r="E129" s="20"/>
-      <c r="F129" s="22"/>
+      <c r="A129" s="29"/>
+      <c r="B129" s="29"/>
+      <c r="C129" s="29"/>
+      <c r="D129" s="19"/>
+      <c r="E129" s="19"/>
+      <c r="F129" s="25"/>
       <c r="G129" s="3" t="s">
         <v>94</v>
       </c>
@@ -3559,12 +3571,12 @@
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="26"/>
-      <c r="B130" s="26"/>
-      <c r="C130" s="26"/>
-      <c r="D130" s="20"/>
-      <c r="E130" s="20"/>
-      <c r="F130" s="22"/>
+      <c r="A130" s="29"/>
+      <c r="B130" s="29"/>
+      <c r="C130" s="29"/>
+      <c r="D130" s="19"/>
+      <c r="E130" s="19"/>
+      <c r="F130" s="25"/>
       <c r="G130" s="5" t="s">
         <v>97</v>
       </c>
@@ -3576,18 +3588,18 @@
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="26">
+      <c r="A131" s="29">
         <v>39</v>
       </c>
-      <c r="B131" s="27">
+      <c r="B131" s="28">
         <v>44855</v>
       </c>
-      <c r="C131" s="26" t="s">
+      <c r="C131" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D131" s="20"/>
-      <c r="E131" s="20"/>
-      <c r="F131" s="22"/>
+      <c r="D131" s="19"/>
+      <c r="E131" s="19"/>
+      <c r="F131" s="25"/>
       <c r="G131" s="9" t="s">
         <v>91</v>
       </c>
@@ -3599,12 +3611,12 @@
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="26"/>
-      <c r="B132" s="26"/>
-      <c r="C132" s="26"/>
-      <c r="D132" s="20"/>
-      <c r="E132" s="20"/>
-      <c r="F132" s="22"/>
+      <c r="A132" s="29"/>
+      <c r="B132" s="29"/>
+      <c r="C132" s="29"/>
+      <c r="D132" s="19"/>
+      <c r="E132" s="19"/>
+      <c r="F132" s="25"/>
       <c r="G132" s="3" t="s">
         <v>94</v>
       </c>
@@ -3616,12 +3628,12 @@
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="26"/>
-      <c r="B133" s="26"/>
-      <c r="C133" s="26"/>
-      <c r="D133" s="21"/>
-      <c r="E133" s="21"/>
-      <c r="F133" s="22"/>
+      <c r="A133" s="29"/>
+      <c r="B133" s="29"/>
+      <c r="C133" s="29"/>
+      <c r="D133" s="20"/>
+      <c r="E133" s="20"/>
+      <c r="F133" s="25"/>
       <c r="G133" s="5" t="s">
         <v>97</v>
       </c>
@@ -3633,22 +3645,22 @@
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="26">
+      <c r="A134" s="29">
         <v>40</v>
       </c>
-      <c r="B134" s="27">
+      <c r="B134" s="28">
         <v>44860</v>
       </c>
-      <c r="C134" s="26" t="s">
+      <c r="C134" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D134" s="19" t="s">
+      <c r="D134" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E134" s="19" t="s">
+      <c r="E134" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F134" s="22"/>
+      <c r="F134" s="25"/>
       <c r="G134" s="9" t="s">
         <v>91</v>
       </c>
@@ -3660,12 +3672,12 @@
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A135" s="26"/>
-      <c r="B135" s="26"/>
-      <c r="C135" s="26"/>
-      <c r="D135" s="20"/>
-      <c r="E135" s="20"/>
-      <c r="F135" s="22"/>
+      <c r="A135" s="29"/>
+      <c r="B135" s="29"/>
+      <c r="C135" s="29"/>
+      <c r="D135" s="19"/>
+      <c r="E135" s="19"/>
+      <c r="F135" s="25"/>
       <c r="G135" s="3" t="s">
         <v>94</v>
       </c>
@@ -3677,12 +3689,12 @@
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A136" s="26"/>
-      <c r="B136" s="26"/>
-      <c r="C136" s="26"/>
-      <c r="D136" s="21"/>
-      <c r="E136" s="21"/>
-      <c r="F136" s="22"/>
+      <c r="A136" s="29"/>
+      <c r="B136" s="29"/>
+      <c r="C136" s="29"/>
+      <c r="D136" s="20"/>
+      <c r="E136" s="20"/>
+      <c r="F136" s="25"/>
       <c r="G136" s="5" t="s">
         <v>97</v>
       </c>
@@ -3718,9 +3730,16 @@
     <mergeCell ref="D79:D82"/>
     <mergeCell ref="D83:D85"/>
     <mergeCell ref="D86:D92"/>
-    <mergeCell ref="A121:A123"/>
-    <mergeCell ref="B121:B123"/>
-    <mergeCell ref="C121:C123"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="A117:A119"/>
+    <mergeCell ref="B117:B119"/>
+    <mergeCell ref="C117:C119"/>
+    <mergeCell ref="A110:A112"/>
+    <mergeCell ref="B110:B112"/>
+    <mergeCell ref="C110:C112"/>
+    <mergeCell ref="A113:A116"/>
+    <mergeCell ref="B113:B116"/>
+    <mergeCell ref="C113:C116"/>
     <mergeCell ref="A73:A75"/>
     <mergeCell ref="B73:B75"/>
     <mergeCell ref="C73:C75"/>
@@ -3747,7 +3766,9 @@
     <mergeCell ref="C134:C136"/>
     <mergeCell ref="D121:D133"/>
     <mergeCell ref="E121:E133"/>
-    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="A121:A123"/>
+    <mergeCell ref="B121:B123"/>
+    <mergeCell ref="C121:C123"/>
     <mergeCell ref="C69:C71"/>
     <mergeCell ref="A66:A68"/>
     <mergeCell ref="B66:B68"/>
@@ -3758,6 +3779,7 @@
     <mergeCell ref="A59:A61"/>
     <mergeCell ref="B59:B61"/>
     <mergeCell ref="C59:C61"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="C45:C48"/>
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="B42:B44"/>
@@ -3772,22 +3794,8 @@
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="B27:B30"/>
     <mergeCell ref="C27:C30"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="B86:B89"/>
     <mergeCell ref="A27:A30"/>
     <mergeCell ref="B24:B26"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D17:D20"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="A14:A16"/>
     <mergeCell ref="A52:A55"/>
     <mergeCell ref="B52:B55"/>
     <mergeCell ref="C52:C55"/>
@@ -3801,10 +3809,17 @@
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="B35:B38"/>
-    <mergeCell ref="E17:E20"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="A14:A16"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="B17:B20"/>
     <mergeCell ref="A24:A26"/>
@@ -3813,28 +3828,13 @@
     <mergeCell ref="A31:A33"/>
     <mergeCell ref="B31:B33"/>
     <mergeCell ref="C31:C33"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
     <mergeCell ref="E27:E33"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="A103:A105"/>
-    <mergeCell ref="B103:B105"/>
-    <mergeCell ref="C103:C105"/>
-    <mergeCell ref="E100:E102"/>
-    <mergeCell ref="E106:E109"/>
-    <mergeCell ref="E110:E112"/>
-    <mergeCell ref="A96:A99"/>
-    <mergeCell ref="B96:B99"/>
-    <mergeCell ref="C96:C99"/>
-    <mergeCell ref="E96:E99"/>
-    <mergeCell ref="A100:A102"/>
-    <mergeCell ref="E103:E105"/>
-    <mergeCell ref="A117:A119"/>
-    <mergeCell ref="B117:B119"/>
-    <mergeCell ref="C117:C119"/>
+    <mergeCell ref="D31:D33"/>
+    <mergeCell ref="D24:D30"/>
+    <mergeCell ref="D17:D20"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E17:E20"/>
+    <mergeCell ref="E21:E23"/>
     <mergeCell ref="A83:A85"/>
     <mergeCell ref="B100:B102"/>
     <mergeCell ref="C100:C102"/>
@@ -3844,12 +3844,8 @@
     <mergeCell ref="A106:A109"/>
     <mergeCell ref="B106:B109"/>
     <mergeCell ref="C106:C109"/>
-    <mergeCell ref="A110:A112"/>
-    <mergeCell ref="B110:B112"/>
-    <mergeCell ref="C110:C112"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="B113:B116"/>
-    <mergeCell ref="C113:C116"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="B86:B89"/>
     <mergeCell ref="A90:A92"/>
     <mergeCell ref="B90:B92"/>
     <mergeCell ref="C90:C92"/>
@@ -3863,13 +3859,18 @@
     <mergeCell ref="D96:D102"/>
     <mergeCell ref="D103:D116"/>
     <mergeCell ref="D118:D119"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="D24:D30"/>
-    <mergeCell ref="D40:D44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="A103:A105"/>
+    <mergeCell ref="B103:B105"/>
+    <mergeCell ref="C103:C105"/>
+    <mergeCell ref="E100:E102"/>
+    <mergeCell ref="E106:E109"/>
+    <mergeCell ref="E110:E112"/>
+    <mergeCell ref="A96:A99"/>
+    <mergeCell ref="B96:B99"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="E96:E99"/>
+    <mergeCell ref="A100:A102"/>
+    <mergeCell ref="E103:E105"/>
     <mergeCell ref="E117:E119"/>
     <mergeCell ref="E39:E41"/>
     <mergeCell ref="E56:E58"/>
@@ -3879,9 +3880,6 @@
     <mergeCell ref="E90:E92"/>
     <mergeCell ref="E93:E95"/>
     <mergeCell ref="E113:E116"/>
-    <mergeCell ref="D56:D61"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D16"/>
     <mergeCell ref="D2:D4"/>
     <mergeCell ref="D35:D39"/>
     <mergeCell ref="F35:F44"/>
@@ -3892,6 +3890,20 @@
     <mergeCell ref="F10:F16"/>
     <mergeCell ref="F17:F33"/>
     <mergeCell ref="D62:D68"/>
+    <mergeCell ref="D40:D44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="D52:D55"/>
+    <mergeCell ref="D56:D61"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="D11:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>